<commit_message>
Update Nowy Arkusz programu Microsoft Excel.xlsx
</commit_message>
<xml_diff>
--- a/4-cycles_and_paths/Nowy Arkusz programu Microsoft Excel.xlsx
+++ b/4-cycles_and_paths/Nowy Arkusz programu Microsoft Excel.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a258678afa0cae05/Documents/Documents 1/GitHub/AiSD_lab/4-cycles_and_paths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA068FF-4408-499A-99AD-BC5FEBC82CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="13_ncr:1_{5EA068FF-4408-499A-99AD-BC5FEBC82CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39E17FB7-193D-42AE-9B30-6D3A9965FD8D}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -26,6 +37,9 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+  <si>
+    <t>liczba_elementów</t>
+  </si>
   <si>
     <t>hamilton_1</t>
   </si>
@@ -39,9 +53,6 @@
     <t>euler</t>
   </si>
   <si>
-    <t>liczba_elementów</t>
-  </si>
-  <si>
     <t>liczba_cykli</t>
   </si>
 </sst>
@@ -49,8 +60,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -103,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -113,12 +125,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -398,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,19 +422,19 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="5">
+      <c r="A1" s="6">
         <v>0.2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2">
         <v>7</v>
@@ -471,167 +486,167 @@
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="5"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>1.3284683227537901E-4</v>
+        <v>1.6541957855224401E-3</v>
       </c>
       <c r="D2" s="4">
-        <v>6.7508697509765497E-3</v>
+        <v>2.3498242950439302E-3</v>
       </c>
       <c r="E2" s="2">
-        <v>9.5599174499511608E-3</v>
+        <v>2.44336128234862E-3</v>
       </c>
       <c r="F2" s="4">
-        <v>7.6556682586669802E-3</v>
+        <v>2.0349550247192299E-2</v>
       </c>
       <c r="G2" s="4">
-        <v>9.4490528106689307E-3</v>
+        <v>1.8458843231201E-3</v>
       </c>
       <c r="H2" s="4">
         <v>9.9053859710693196E-3</v>
       </c>
       <c r="I2" s="1">
-        <v>6.5706253051757701E-3</v>
+        <v>9.5475196838378795E-3</v>
       </c>
       <c r="J2" s="1">
-        <v>3.5591602325439299E-3</v>
+        <v>3.8240432739257701E-3</v>
       </c>
       <c r="K2" s="1">
-        <v>1.54524326324462E-2</v>
+        <v>0.14388327598571701</v>
       </c>
       <c r="L2" s="1">
-        <v>1.4232683181762599E-2</v>
+        <v>3.2932567596435501E-2</v>
       </c>
       <c r="M2" s="1">
-        <v>1.95146083831787E-2</v>
+        <v>5.5526542663574201E-2</v>
       </c>
       <c r="N2" s="1">
-        <v>2.2475290298461899E-2</v>
+        <v>1.3637590408325099E-2</v>
       </c>
       <c r="O2" s="1">
-        <v>2.10500240325927E-2</v>
+        <v>2.0345735549926702E-2</v>
       </c>
       <c r="P2" s="1">
-        <v>2.66914844512939E-2</v>
+        <v>1.46167755126953E-2</v>
       </c>
       <c r="Q2" s="1">
-        <v>1.84255123138427E-2</v>
+        <v>3.47493171691894E-2</v>
       </c>
       <c r="R2" s="2">
-        <v>4.2475271224975499E-2</v>
+        <v>3.4063148498535097E-2</v>
       </c>
     </row>
     <row r="3" spans="1:18">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>2.5942802429199099E-3</v>
+        <v>1.9693851470947098E-3</v>
       </c>
       <c r="D3" s="4">
-        <v>3.76610755920409E-3</v>
+        <v>1.0772752761840801E-2</v>
       </c>
       <c r="E3" s="4">
-        <v>1.52721881866454E-2</v>
+        <v>3.1683921813964698E-3</v>
       </c>
       <c r="F3" s="3">
-        <v>7.9441070556629496E-5</v>
+        <v>2.1059083938598601E-2</v>
       </c>
       <c r="G3" s="4">
-        <v>2.3415565490722502E-3</v>
+        <v>2.12767601013183E-2</v>
       </c>
       <c r="H3" s="4">
         <v>3.3122348785400303E-2</v>
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="A4" s="5"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
       <c r="G4" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>1.53034210205078E-2</v>
+        <v>3.12614440917957E-4</v>
       </c>
       <c r="D5" s="4">
-        <v>8.5167884826659003E-4</v>
+        <v>3.3574104309080899E-4</v>
       </c>
       <c r="E5" s="4">
-        <v>1.47812843322753E-2</v>
+        <v>3.1571388244627698E-4</v>
       </c>
       <c r="F5" s="4">
-        <v>1.40981674194334E-3</v>
+        <v>3.2382011413573098E-4</v>
       </c>
       <c r="G5" s="4">
         <v>1.7838954925536901E-3</v>
       </c>
       <c r="H5" s="4">
-        <v>1.02429389953612E-3</v>
+        <v>3.6697387695311298E-4</v>
       </c>
       <c r="I5" s="2">
-        <v>1.47085189819334E-3</v>
+        <v>2.42519378662098E-4</v>
       </c>
       <c r="J5" s="2">
-        <v>1.6623020172118999E-3</v>
+        <v>1.7099380493162901E-4</v>
       </c>
       <c r="K5" s="1">
-        <v>2.6314735412597502E-3</v>
+        <v>2.5634765624998798E-4</v>
       </c>
       <c r="L5" s="1">
-        <v>1.64608955383299E-3</v>
+        <v>2.5086402893065198E-4</v>
       </c>
       <c r="M5" s="2">
-        <v>2.6698589324951E-3</v>
+        <v>1.73854827880848E-4</v>
       </c>
       <c r="N5" s="1">
-        <v>2.0053863525390501E-3</v>
+        <v>3.1309127807616001E-4</v>
       </c>
       <c r="O5" s="1">
-        <v>2.5701999664306499E-3</v>
+        <v>3.1213760375975398E-4</v>
       </c>
       <c r="P5" s="1">
-        <v>4.6349048614501799E-3</v>
+        <v>3.88908386230457E-4</v>
       </c>
       <c r="Q5" s="1">
-        <v>9.4256877899169794E-3</v>
+        <v>3.8080215454100398E-4</v>
       </c>
       <c r="R5" s="1">
-        <v>2.38707542419433E-2</v>
+        <v>3.9558410644530102E-4</v>
       </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>0.6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>7</v>
@@ -683,159 +698,159 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>2.6682901382446202E-2</v>
+        <v>6.55937194824207E-4</v>
       </c>
       <c r="D7" s="4">
-        <v>1.32851600646971E-3</v>
+        <v>1.2016773223876801E-3</v>
       </c>
       <c r="E7" s="4">
-        <v>3.1137943267822098E-3</v>
+        <v>1.80249214172362E-3</v>
       </c>
       <c r="F7" s="4">
-        <v>1.7333078384399399E-2</v>
+        <v>1.4551162719726399E-3</v>
       </c>
       <c r="G7" s="4">
-        <v>1.8935680389404099E-3</v>
+        <v>2.1126747131347502E-3</v>
       </c>
       <c r="H7" s="4">
         <v>1.7009305953979401E-2</v>
       </c>
       <c r="I7" s="1">
-        <v>2.5904655456542801E-3</v>
+        <v>4.8575878143310401E-3</v>
       </c>
       <c r="J7" s="1">
-        <v>1.6946601867675701E-2</v>
+        <v>3.4144401550292801E-3</v>
       </c>
       <c r="K7" s="1">
-        <v>1.6660499572753801E-2</v>
+        <v>5.8415412902831903E-3</v>
       </c>
       <c r="L7" s="1">
-        <v>1.8470096588134699E-2</v>
+        <v>1.33600711822509E-2</v>
       </c>
       <c r="M7" s="1">
-        <v>1.7850208282470598E-2</v>
+        <v>1.2358713150024399E-2</v>
       </c>
       <c r="N7" s="1">
-        <v>1.84865474700927E-2</v>
+        <v>1.0268735885620099E-2</v>
       </c>
       <c r="O7" s="1">
-        <v>1.86474800109863E-2</v>
+        <v>1.4494228363036999E-2</v>
       </c>
       <c r="P7" s="2">
-        <v>1.7962026596069301E-2</v>
+        <v>1.76883220672607E-2</v>
       </c>
       <c r="Q7" s="1">
-        <v>2.5801706314086899E-2</v>
+        <v>1.9932794570922799E-2</v>
       </c>
       <c r="R7" s="1">
-        <v>2.27263450622558E-2</v>
+        <v>2.2589731216430601E-2</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>2.1779108047485299E-2</v>
+        <v>6.3315916061401301E-2</v>
       </c>
       <c r="D8" s="4">
-        <v>0.12509684562683099</v>
+        <v>0.31706719398498501</v>
       </c>
       <c r="E8" s="4">
-        <v>0.32717304229736299</v>
+        <v>1.1945293426513599</v>
       </c>
       <c r="F8" s="4">
-        <v>3.7772307872772202</v>
+        <v>13.939061212539601</v>
       </c>
       <c r="G8" s="4">
-        <v>22.5832605838775</v>
+        <v>134.77617983818001</v>
       </c>
       <c r="H8" s="4">
         <v>337.27851395606899</v>
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="5"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2">
-        <v>80</v>
+        <v>336</v>
       </c>
       <c r="D9" s="2">
-        <v>912</v>
+        <v>1164</v>
       </c>
       <c r="E9" s="4">
-        <v>1872</v>
+        <v>3180</v>
       </c>
       <c r="F9" s="2">
-        <v>23568</v>
+        <v>41908</v>
       </c>
       <c r="G9" s="4">
-        <v>115788</v>
+        <v>322416</v>
       </c>
       <c r="H9" s="4">
         <v>1308044</v>
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>6.7761421203613101E-3</v>
+        <v>4</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2.65407562255848E-4</v>
       </c>
       <c r="D10" s="4">
-        <v>9.1581344604491001E-4</v>
+        <v>2.5181770324705899E-4</v>
       </c>
       <c r="E10" s="4">
-        <v>2.35300064086912E-3</v>
+        <v>3.1833648681639499E-4</v>
       </c>
       <c r="F10" s="4">
-        <v>1.6634941101074099E-3</v>
+        <v>2.8996467590330899E-4</v>
       </c>
       <c r="G10" s="4">
         <v>1.9894123077392402E-3</v>
       </c>
       <c r="H10" s="4">
-        <v>1.8945217132568201E-3</v>
+        <v>2.5324821472166799E-4</v>
       </c>
       <c r="I10" s="1">
-        <v>4.9691200256346503E-4</v>
+        <v>2.6087760925291799E-4</v>
       </c>
       <c r="J10" s="1">
-        <v>3.00674438476561E-3</v>
+        <v>2.8018951416014499E-4</v>
       </c>
       <c r="K10" s="1">
-        <v>2.0714282989501799E-3</v>
+        <v>2.8853416442869902E-4</v>
       </c>
       <c r="L10" s="1">
-        <v>2.7380466461181499E-3</v>
+        <v>2.6421546936034003E-4</v>
       </c>
       <c r="M10" s="2">
-        <v>1.82834148406982E-2</v>
+        <v>3.5934448242186298E-4</v>
       </c>
       <c r="N10" s="1">
-        <v>1.8288898468017501E-2</v>
+        <v>3.6029815673826999E-4</v>
       </c>
       <c r="O10" s="1">
-        <v>1.7654228210449201E-2</v>
+        <v>3.2167434692381702E-4</v>
       </c>
       <c r="P10" s="1">
-        <v>1.6461420059204E-2</v>
+        <v>2.63023376464832E-4</v>
       </c>
       <c r="Q10" s="1">
-        <v>3.96736145019531E-2</v>
+        <v>3.1189918518065198E-4</v>
       </c>
       <c r="R10" s="1">
-        <v>4.1550683975219702E-2</v>
+        <v>3.81278991699207E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>